<commit_message>
Update Excel document for the comments. Changed /v1/record-service-request :: Request body completenes, /v1/record-service-request :: Attribute configured? and /v1/list-records, /v1/list-records-of-flow and /v1/list-records-of-unsuccessful, Response body completeness
</commit_message>
<xml_diff>
--- a/testing/EaTL+testcase.docs.xlsx
+++ b/testing/EaTL+testcase.docs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\Documents\MW\EaTL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW_Testing\EaTL_Documentation\ExecutionAndTraceLog\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E4661E-9D94-4465-91AC-F1A3CA75ADDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909E80C0-F385-42E8-9B21-EF5720F263AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="233">
   <si>
     <t>Testcases</t>
   </si>
@@ -1261,12 +1261,6 @@
 </t>
   </si>
   <si>
-    <t>#### Testing:
-- checking for ResponseCode==204
-- GETing CC (/core-model-1-4:control-construct)
-- searching CC for service-record-profile of x-correlator=dummyXCorrelator</t>
-  </si>
-  <si>
     <t>/v1/list-records-of-flow</t>
   </si>
   <si>
@@ -1399,6 +1393,25 @@
    - new-application-protocol, new-application-address and new-application-port with random generated dummy values (assure sufficiently high probability that set does not exist!)
    - operation-key from above
    - reasonable parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#### Testing:
+- Checking for response-code 200
+- checking the response body for each attribute against the specification
+</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- Checking for response-code 200
+- checking the response body for each attribute against the specification</t>
+  </si>
+  <si>
+    <t>#### Testing:
+- checking for ResponseCode==204 for /v1/record-service-request
+- POST /v1//v1/list-records-of-flow and store response
+  - verify that received response parameters is equal to expected attribute values 
+  ex: application-name == ExpectedApplicationName, release-number ==   expectedReleaseNumber, operation-name == expectedOperationName, 
+response-code = expectedResponseCode, similarly other parameters.</t>
   </si>
 </sst>
 </file>
@@ -2199,10 +2212,10 @@
   <dimension ref="A1:J229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="H58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C158" sqref="C158"/>
+      <selection pane="bottomRight" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2270,10 +2283,10 @@
         <v>201</v>
       </c>
       <c r="I3" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>216</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -2322,7 +2335,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D5" s="21" t="str">
         <f>CONCATENATE("#### Preparation:
@@ -2472,13 +2485,13 @@
         <v>208</v>
       </c>
       <c r="H6" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I6" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J6" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
@@ -5175,19 +5188,19 @@
         <v>90</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G52" t="s">
         <v>90</v>
       </c>
       <c r="H52" s="51" t="s">
-        <v>46</v>
+        <v>231</v>
       </c>
       <c r="I52" s="51" t="s">
-        <v>46</v>
+        <v>230</v>
       </c>
       <c r="J52" s="51" t="s">
-        <v>46</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -5728,14 +5741,14 @@
   - searching CC for op-s of ",G3,", storing operation-key")
 &amp;CONCATENATE("
 - POST ",G3,"
-   - all attributes filled with random values
+   - all attributes filled with random values BUT one randomly chosen attribute missing
     -operation-key from above
     - reasonable parameters")</f>
         <v>#### Preparation:
 - GETing CC (/core-model-1-4:control-construct)
   - searching CC for op-s of /v1/record-service-request, storing operation-key
 - POST /v1/record-service-request
-   - all attributes filled with random values
+   - all attributes filled with random values BUT one randomly chosen attribute missing
     -operation-key from above
     - reasonable parameters</v>
       </c>
@@ -6542,7 +6555,7 @@
         <v>90</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6610,7 +6623,7 @@
         <v>156</v>
       </c>
       <c r="D101" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E101" s="21"/>
       <c r="F101" s="52" t="s">
@@ -6685,7 +6698,7 @@
         <v>160</v>
       </c>
       <c r="D106" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6735,7 +6748,7 @@
         <v>159</v>
       </c>
       <c r="D111" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6877,7 +6890,7 @@
         <v>191</v>
       </c>
       <c r="D123" s="44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E123" s="43" t="s">
         <v>90</v>
@@ -6967,7 +6980,7 @@
         <v>90</v>
       </c>
       <c r="D127" s="39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E127" s="39" t="s">
         <v>110</v>
@@ -7009,10 +7022,10 @@
         <v>90</v>
       </c>
       <c r="D129" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E129" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F129" s="39" t="s">
         <v>90</v>
@@ -7210,7 +7223,7 @@
         <v>188</v>
       </c>
       <c r="D141" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E141" s="39" t="s">
         <v>90</v>
@@ -7285,7 +7298,7 @@
         <v>189</v>
       </c>
       <c r="D147" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
@@ -7345,7 +7358,7 @@
         <v>175</v>
       </c>
       <c r="D153" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
@@ -7914,6 +7927,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A183:A189"/>
     <mergeCell ref="A59:A62"/>
@@ -7929,16 +7952,6 @@
     <mergeCell ref="A170:A176"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
findings in test-suite Fixes #226
</commit_message>
<xml_diff>
--- a/testing/EaTL+testcase.docs.xlsx
+++ b/testing/EaTL+testcase.docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venka\MW_Testing\EaTL_Documentation\ExecutionAndTraceLog\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IS00759329\Desktop\Telefonica\ApplicationPattern\ApplicationPattern_v2\testSuites_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8C700C-E8A9-49BB-B99B-3BC902437B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0A7FBF-02AD-42EA-9628-5677A2141BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
+    <workbookView xWindow="285" yWindow="270" windowWidth="20205" windowHeight="10650" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Servicelayer" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="234">
   <si>
     <t>Testcases</t>
   </si>
@@ -1412,6 +1412,14 @@
   - verify that received response parameters is equal to expected attribute values 
   ex: application-name == ExpectedApplicationName, release-number ==   expectedReleaseNumber, operation-name == expectedOperationName, 
 response-code = expectedResponseCode, similarly other parameters.</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+ - PUT initial newRelease/application-name
+- PUT initial newRelease/release-number
+- PUT initial newRelease/protocol
+- PUT initial newRelease/address
+- PUT initial newRelease/port</t>
   </si>
 </sst>
 </file>
@@ -2211,27 +2219,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6438CD8-A3F3-4ED1-9D84-D5D573F05C15}">
   <dimension ref="A1:J229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="F94" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G97" sqref="G97"/>
+      <selection pane="bottomRight" activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="58" customWidth="1"/>
-    <col min="2" max="2" width="70.7265625" style="2"/>
-    <col min="3" max="6" width="70.7265625" style="52"/>
-    <col min="7" max="7" width="70.7265625" style="52" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" style="2"/>
+    <col min="3" max="6" width="70.7109375" style="52"/>
+    <col min="7" max="7" width="70.7109375" style="52" customWidth="1"/>
     <col min="8" max="8" width="70" style="52" customWidth="1"/>
-    <col min="9" max="9" width="63.36328125" style="52" customWidth="1"/>
-    <col min="10" max="10" width="64.36328125" style="52" customWidth="1"/>
-    <col min="11" max="40" width="9.1796875" style="52" customWidth="1"/>
-    <col min="41" max="16384" width="9.1796875" style="52"/>
+    <col min="9" max="9" width="63.42578125" style="52" customWidth="1"/>
+    <col min="10" max="10" width="64.42578125" style="52" customWidth="1"/>
+    <col min="11" max="40" width="9.140625" style="52" customWidth="1"/>
+    <col min="41" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>206</v>
       </c>
@@ -2242,7 +2250,7 @@
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
     </row>
-    <row r="2" spans="1:10" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
@@ -2257,7 +2265,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
@@ -2289,7 +2297,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>3</v>
       </c>
@@ -2329,7 +2337,7 @@
         <v>## Is service idempotent?</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A5" s="64"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -2453,7 +2461,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="64"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -2494,7 +2502,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
@@ -2538,7 +2546,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
         <v>8</v>
       </c>
@@ -2578,7 +2586,7 @@
         <v>## Get parameters checked for completeness?</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="64"/>
       <c r="B9" s="8" t="s">
         <v>10</v>
@@ -2700,7 +2708,7 @@
     -  BUT one randomly chosen parameter (user, originator, x-correlator, trace-indicator or customer-journey) missing (not empty string!)</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="64"/>
       <c r="B10" s="8" t="s">
         <v>11</v>
@@ -2746,7 +2754,7 @@
 - checking for ResponseCode == 400</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="64"/>
       <c r="B11" s="6" t="str">
         <f>$B7</f>
@@ -2792,7 +2800,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>12</v>
       </c>
@@ -2832,7 +2840,7 @@
         <v>## Gets originator checked for compliance with specification?</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="64"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
@@ -2954,7 +2962,7 @@
           1.  originator set to be a string of 0, 1 or 2 (random) letters length (too short).</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="64"/>
       <c r="B14" s="8" t="s">
         <v>15</v>
@@ -3000,7 +3008,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="64"/>
       <c r="B15" s="6" t="str">
         <f>$B7</f>
@@ -3046,7 +3054,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="64" t="s">
         <v>16</v>
       </c>
@@ -3086,7 +3094,7 @@
         <v>## Gets x-correlator checked for complying the pattern?</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A17" s="64"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
@@ -3208,7 +3216,7 @@
     - reasonable parameters, BUT dummyXCorrelators differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="64"/>
       <c r="B18" s="8" t="s">
         <v>15</v>
@@ -3254,7 +3262,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="64"/>
       <c r="B19" s="6" t="str">
         <f>$B7</f>
@@ -3300,7 +3308,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="64" t="s">
         <v>19</v>
       </c>
@@ -3340,7 +3348,7 @@
         <v>## Gets trace-indicator checked for complying the pattern?</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A21" s="64"/>
       <c r="B21" s="8" t="s">
         <v>21</v>
@@ -3462,7 +3470,7 @@
     - reasonable parameters, BUT dummyTraceIndicator differing from the pattern in various ways (e.g. empty string)</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="64"/>
       <c r="B22" s="8" t="s">
         <v>15</v>
@@ -3508,7 +3516,7 @@
 - checking for ResponseCode==400</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="64"/>
       <c r="B23" s="6" t="str">
         <f>$B7</f>
@@ -3554,7 +3562,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="64" t="s">
         <v>22</v>
       </c>
@@ -3594,7 +3602,7 @@
         <v>## Gets security key checked for availability?</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A25" s="64"/>
       <c r="B25" s="8" t="s">
         <v>24</v>
@@ -3690,7 +3698,7 @@
     - BUT operationKey parameter missing (does not mean empty string)</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="64"/>
       <c r="B26" s="8" t="s">
         <v>25</v>
@@ -3736,7 +3744,7 @@
 - checking for ResponseCode==401</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="64"/>
       <c r="B27" s="6" t="str">
         <f>$B7</f>
@@ -3782,7 +3790,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="64" t="s">
         <v>26</v>
       </c>
@@ -3822,7 +3830,7 @@
         <v>## Gets security key checked for correctness?</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A29" s="64"/>
       <c r="B29" s="8" t="s">
         <v>28</v>
@@ -3918,7 +3926,7 @@
      - BUT operationKey parameter with random dummy value</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="64"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
@@ -3964,7 +3972,7 @@
 - checking for ResponseCode==401</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="64"/>
       <c r="B31" s="6" t="str">
         <f>$B7</f>
@@ -4010,7 +4018,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="64" t="s">
         <v>29</v>
       </c>
@@ -4050,7 +4058,7 @@
         <v>## Contains response complete set of headers?</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A33" s="64"/>
       <c r="B33" s="8" t="s">
         <v>31</v>
@@ -4135,7 +4143,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="64"/>
       <c r="B34" s="8" t="s">
         <v>32</v>
@@ -4171,7 +4179,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="64"/>
       <c r="B35" s="6" t="str">
         <f>$B7</f>
@@ -4217,7 +4225,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="64" t="s">
         <v>33</v>
       </c>
@@ -4257,7 +4265,7 @@
         <v>## Is the initial x-correlator ín the response?</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A37" s="64"/>
       <c r="B37" s="8" t="s">
         <v>31</v>
@@ -4342,7 +4350,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="64"/>
       <c r="B38" s="8" t="s">
         <v>35</v>
@@ -4381,7 +4389,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="64"/>
       <c r="B39" s="6" t="str">
         <f>$B7</f>
@@ -4427,7 +4435,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="64" t="s">
         <v>36</v>
       </c>
@@ -4467,7 +4475,7 @@
         <v>## Is the correct life-cycle-state ín the response?</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A41" s="65"/>
       <c r="B41" s="8" t="s">
         <v>31</v>
@@ -4552,7 +4560,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="65"/>
       <c r="B42" s="8" t="s">
         <v>38</v>
@@ -4622,7 +4630,7 @@
 - checking for response headers containing life-cycle-state is equal to the value as present in the control-construct for /v1/list-records-of-unsuccessful/configuration/life-cycle-state</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="65"/>
       <c r="B43" s="6" t="str">
         <f>$B7</f>
@@ -4668,7 +4676,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
         <v>39</v>
       </c>
@@ -4700,7 +4708,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="65"/>
       <c r="B45" s="8" t="s">
         <v>41</v>
@@ -4730,7 +4738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A46" s="65"/>
       <c r="B46" s="8" t="s">
         <v>182</v>
@@ -4888,7 +4896,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" s="65"/>
       <c r="B47" s="8" t="s">
         <v>183</v>
@@ -5009,7 +5017,7 @@
    - checking same record for containing DummyXCorrelator &amp;DummyTraceIndicator</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="65"/>
       <c r="B48" s="9" t="str">
         <f>$B7</f>
@@ -5053,7 +5061,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="56" t="s">
         <v>42</v>
       </c>
@@ -5067,7 +5075,7 @@
       <c r="I49" s="62"/>
       <c r="J49" s="62"/>
     </row>
-    <row r="50" spans="1:10" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="66" t="s">
         <v>43</v>
       </c>
@@ -5099,7 +5107,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="64"/>
       <c r="B51" s="12" t="s">
         <v>45</v>
@@ -5173,7 +5181,7 @@
       - reasonable parameters </v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="64"/>
       <c r="B52" s="13" t="s">
         <v>46</v>
@@ -5203,7 +5211,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="64"/>
       <c r="B53" s="14" t="s">
         <v>47</v>
@@ -5241,7 +5249,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="65" t="s">
         <v>48</v>
       </c>
@@ -5273,7 +5281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="174" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="65"/>
       <c r="B55" s="12" t="s">
         <v>50</v>
@@ -5324,7 +5332,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="65"/>
       <c r="B56" s="13" t="s">
         <v>51</v>
@@ -5354,7 +5362,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="65"/>
       <c r="B57" s="14" t="s">
         <v>47</v>
@@ -5384,7 +5392,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="65"/>
       <c r="B58" s="13" t="s">
         <v>52</v>
@@ -5412,7 +5420,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="64" t="s">
         <v>53</v>
       </c>
@@ -5452,7 +5460,7 @@
         <v>## Gets lifeCycleState propagated?</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A60" s="65"/>
       <c r="B60" s="8" t="s">
         <v>55</v>
@@ -5588,7 +5596,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="65"/>
       <c r="B61" s="8" t="s">
         <v>56</v>
@@ -5618,7 +5626,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="65"/>
       <c r="B62" s="15" t="s">
         <v>57</v>
@@ -5648,7 +5656,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="64" t="s">
         <v>58</v>
       </c>
@@ -5688,7 +5696,7 @@
         <v>## Get attributes checked for completeness?</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A64" s="64"/>
       <c r="B64" s="8" t="s">
         <v>60</v>
@@ -5762,7 +5770,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="64"/>
       <c r="B65" s="8" t="s">
         <v>61</v>
@@ -5798,7 +5806,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="64"/>
       <c r="B66" s="15" t="s">
         <v>47</v>
@@ -5836,7 +5844,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="64" t="s">
         <v>130</v>
       </c>
@@ -5876,7 +5884,7 @@
         <v>## Get each attributes checked for correctness?</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="64"/>
       <c r="B68" s="8"/>
       <c r="C68" s="41" t="s">
@@ -5898,7 +5906,7 @@
       <c r="I68"/>
       <c r="J68"/>
     </row>
-    <row r="69" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A69" s="64"/>
       <c r="B69" s="8"/>
       <c r="C69" s="21" t="s">
@@ -5960,7 +5968,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="64"/>
       <c r="B70" s="8"/>
       <c r="C70" s="25" t="str">
@@ -5987,7 +5995,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="64"/>
       <c r="B71" s="8"/>
       <c r="C71" s="22" t="str">
@@ -6020,7 +6028,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="64"/>
       <c r="B72" s="8"/>
       <c r="C72" s="41" t="s">
@@ -6042,7 +6050,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A73" s="64"/>
       <c r="B73" s="8"/>
       <c r="C73" s="21" t="s">
@@ -6085,7 +6093,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="64"/>
       <c r="B74" s="8"/>
       <c r="C74" s="25" t="str">
@@ -6102,7 +6110,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="64"/>
       <c r="B75" s="8"/>
       <c r="C75" s="50" t="str">
@@ -6121,7 +6129,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="64"/>
       <c r="B76" s="8"/>
       <c r="C76" s="41" t="s">
@@ -6134,7 +6142,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="203" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A77" s="64"/>
       <c r="B77" s="8"/>
       <c r="C77" s="21" t="s">
@@ -6177,7 +6185,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="64"/>
       <c r="B78" s="8"/>
       <c r="C78" s="25" t="str">
@@ -6194,7 +6202,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="64"/>
       <c r="B79" s="8"/>
       <c r="C79" s="22" t="str">
@@ -6213,7 +6221,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="64"/>
       <c r="B80" s="8"/>
       <c r="C80" s="41" t="s">
@@ -6226,7 +6234,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A81" s="64"/>
       <c r="B81" s="8"/>
       <c r="C81" s="21" t="s">
@@ -6269,7 +6277,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="64"/>
       <c r="B82" s="8"/>
       <c r="C82" s="25" t="str">
@@ -6286,7 +6294,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="64"/>
       <c r="B83" s="8"/>
       <c r="C83" s="22" t="str">
@@ -6305,7 +6313,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="64"/>
       <c r="B84" s="8"/>
       <c r="C84" s="22"/>
@@ -6316,7 +6324,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A85" s="64"/>
       <c r="B85" s="8"/>
       <c r="C85" s="22"/>
@@ -6357,7 +6365,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="64"/>
       <c r="B86" s="8"/>
       <c r="C86" s="22"/>
@@ -6370,7 +6378,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="64"/>
       <c r="B87" s="8"/>
       <c r="C87" s="22"/>
@@ -6385,7 +6393,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="64"/>
       <c r="B88" s="8"/>
       <c r="C88" s="22"/>
@@ -6394,7 +6402,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="64"/>
       <c r="B89" s="8"/>
       <c r="C89" s="22"/>
@@ -6417,7 +6425,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="64"/>
       <c r="B90" s="8"/>
       <c r="C90" s="22"/>
@@ -6426,7 +6434,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="64"/>
       <c r="B91" s="8"/>
       <c r="C91" s="22"/>
@@ -6437,7 +6445,7 @@
 - not applicable</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="64"/>
       <c r="B92" s="8"/>
       <c r="C92" s="22"/>
@@ -6446,7 +6454,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="64"/>
       <c r="B93" s="8"/>
       <c r="C93" s="22"/>
@@ -6469,7 +6477,7 @@
     - reasonable parameters</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="64" t="s">
         <v>63</v>
       </c>
@@ -6497,7 +6505,7 @@
         <v>## Get each attributes checked if getting correctly updated?</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="64"/>
       <c r="B95" s="8"/>
       <c r="C95" s="41" t="s">
@@ -6516,7 +6524,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="232" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A96" s="65"/>
       <c r="B96" s="8" t="s">
         <v>65</v>
@@ -6537,7 +6545,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="65"/>
       <c r="B97" s="8" t="s">
         <v>66</v>
@@ -6558,7 +6566,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="65"/>
       <c r="B98" s="8" t="s">
         <v>47</v>
@@ -6579,7 +6587,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A99" s="55"/>
       <c r="B99" s="13" t="s">
         <v>52</v>
@@ -6597,7 +6605,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="64"/>
       <c r="B100" s="8"/>
       <c r="C100" s="41" t="s">
@@ -6614,7 +6622,7 @@
       </c>
       <c r="G100" s="41"/>
     </row>
-    <row r="101" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="65"/>
       <c r="B101" s="8" t="s">
         <v>65</v>
@@ -6633,7 +6641,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A102" s="65"/>
       <c r="B102" s="8" t="s">
         <v>66</v>
@@ -6650,7 +6658,7 @@
       </c>
       <c r="G102" s="25"/>
     </row>
-    <row r="103" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" s="65"/>
       <c r="B103" s="8" t="s">
         <v>47</v>
@@ -6667,7 +6675,7 @@
       </c>
       <c r="G103" s="22"/>
     </row>
-    <row r="104" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="55"/>
       <c r="B104" s="13" t="s">
         <v>52</v>
@@ -6681,7 +6689,7 @@
       <c r="E104" s="24"/>
       <c r="G104" s="24"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="55"/>
       <c r="B105" s="8"/>
       <c r="C105" s="41" t="s">
@@ -6691,7 +6699,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A106" s="55"/>
       <c r="B106" s="8"/>
       <c r="C106" s="21" t="s">
@@ -6701,7 +6709,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A107" s="55"/>
       <c r="B107" s="8"/>
       <c r="C107" s="25" t="s">
@@ -6711,7 +6719,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="55"/>
       <c r="B108" s="8"/>
       <c r="C108" s="22" t="s">
@@ -6721,7 +6729,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A109" s="55"/>
       <c r="B109" s="8"/>
       <c r="C109" s="24" t="s">
@@ -6731,7 +6739,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="55"/>
       <c r="B110" s="8"/>
       <c r="C110" s="41" t="s">
@@ -6741,7 +6749,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A111" s="55"/>
       <c r="B111" s="8"/>
       <c r="C111" s="21" t="s">
@@ -6751,7 +6759,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A112" s="55"/>
       <c r="B112" s="8"/>
       <c r="C112" s="25" t="s">
@@ -6761,7 +6769,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="55"/>
       <c r="B113" s="8"/>
       <c r="C113" s="22" t="s">
@@ -6771,7 +6779,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A114" s="55"/>
       <c r="B114" s="8"/>
       <c r="C114" s="24" t="s">
@@ -6781,42 +6789,42 @@
         <v>102</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="55"/>
       <c r="B115" s="8"/>
       <c r="C115" s="41" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A116" s="55"/>
       <c r="B116" s="8"/>
       <c r="C116" s="21" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A117" s="55"/>
       <c r="B117" s="8"/>
       <c r="C117" s="25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="55"/>
       <c r="B118" s="8"/>
       <c r="C118" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A119" s="55"/>
       <c r="B119" s="8"/>
       <c r="C119" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="64" t="s">
         <v>67</v>
       </c>
@@ -6839,7 +6847,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="64"/>
       <c r="B121" s="12"/>
       <c r="C121" s="42" t="s">
@@ -6856,7 +6864,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="65"/>
       <c r="B122" s="8" t="s">
         <v>69</v>
@@ -6881,7 +6889,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" ht="330" x14ac:dyDescent="0.25">
       <c r="A123" s="65"/>
       <c r="B123" s="8" t="s">
         <v>190</v>
@@ -6902,7 +6910,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A124" s="65"/>
       <c r="B124" s="8" t="s">
         <v>184</v>
@@ -6923,17 +6931,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A125" s="65"/>
       <c r="B125" s="5" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
-      <c r="C125" s="45" t="str">
-        <f>$B7</f>
-        <v>#### Clearing:
-- not applicable</v>
+      <c r="C125" s="45" t="s">
+        <v>233</v>
       </c>
       <c r="D125" s="45" t="str">
         <f>$B7</f>
@@ -6950,7 +6956,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="64" t="s">
         <v>70</v>
       </c>
@@ -6973,7 +6979,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="64"/>
       <c r="B127" s="13"/>
       <c r="C127" s="39" t="s">
@@ -6992,7 +6998,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A128" s="64"/>
       <c r="B128" s="12" t="s">
         <v>72</v>
@@ -7013,7 +7019,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A129" s="64"/>
       <c r="B129" s="13" t="s">
         <v>73</v>
@@ -7034,7 +7040,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="64"/>
       <c r="B130" s="13" t="s">
         <v>47</v>
@@ -7047,7 +7053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A131" s="64"/>
       <c r="B131" s="13" t="s">
         <v>52</v>
@@ -7060,7 +7066,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="64" t="s">
         <v>74</v>
       </c>
@@ -7083,7 +7089,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="64"/>
       <c r="B133" s="8"/>
       <c r="C133" s="41" t="s">
@@ -7102,7 +7108,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="64"/>
       <c r="B134" s="8" t="s">
         <v>41</v>
@@ -7123,7 +7129,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="290" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A135" s="64"/>
       <c r="B135" s="8" t="s">
         <v>185</v>
@@ -7144,7 +7150,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A136" s="64"/>
       <c r="B136" s="8" t="s">
         <v>187</v>
@@ -7156,7 +7162,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A137" s="64"/>
       <c r="B137" s="8" t="s">
         <v>47</v>
@@ -7168,7 +7174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="64"/>
       <c r="B138" s="13" t="s">
         <v>52</v>
@@ -7180,7 +7186,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="64"/>
       <c r="B139" s="8"/>
       <c r="C139" s="41" t="s">
@@ -7196,7 +7202,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="64"/>
       <c r="B140" s="8" t="s">
         <v>41</v>
@@ -7214,7 +7220,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="290" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" ht="345" x14ac:dyDescent="0.25">
       <c r="A141" s="64"/>
       <c r="B141" s="8" t="s">
         <v>185</v>
@@ -7232,7 +7238,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A142" s="64"/>
       <c r="B142" s="8" t="s">
         <v>187</v>
@@ -7244,7 +7250,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="64"/>
       <c r="B143" s="8" t="s">
         <v>47</v>
@@ -7256,7 +7262,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="64"/>
       <c r="B144" s="13" t="s">
         <v>52</v>
@@ -7268,7 +7274,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="64"/>
       <c r="B145" s="8"/>
       <c r="C145" s="41" t="s">
@@ -7281,7 +7287,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="64"/>
       <c r="B146" s="8"/>
       <c r="C146" s="31" t="s">
@@ -7291,7 +7297,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A147" s="64"/>
       <c r="B147" s="8"/>
       <c r="C147" s="21" t="s">
@@ -7301,7 +7307,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A148" s="64"/>
       <c r="B148" s="8"/>
       <c r="C148" s="29" t="s">
@@ -7311,7 +7317,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="64"/>
       <c r="B149" s="8"/>
       <c r="C149" s="22" t="s">
@@ -7321,7 +7327,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A150" s="64"/>
       <c r="B150" s="8"/>
       <c r="C150" s="24" t="s">
@@ -7331,7 +7337,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="64"/>
       <c r="B151" s="8"/>
       <c r="C151" s="41" t="s">
@@ -7341,7 +7347,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="64"/>
       <c r="B152" s="8"/>
       <c r="C152" s="31" t="s">
@@ -7351,7 +7357,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A153" s="64"/>
       <c r="B153" s="8"/>
       <c r="C153" s="21" t="s">
@@ -7361,7 +7367,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A154" s="64"/>
       <c r="B154" s="8"/>
       <c r="C154" s="29" t="s">
@@ -7371,7 +7377,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="64"/>
       <c r="B155" s="8"/>
       <c r="C155" s="22" t="s">
@@ -7381,7 +7387,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="64"/>
       <c r="B156" s="8"/>
       <c r="C156" s="24" t="s">
@@ -7391,49 +7397,49 @@
         <v>102</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="64"/>
       <c r="B157" s="8"/>
       <c r="C157" s="41" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="64"/>
       <c r="B158" s="8"/>
       <c r="C158" s="31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A159" s="64"/>
       <c r="B159" s="8"/>
       <c r="C159" s="21" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A160" s="64"/>
       <c r="B160" s="8"/>
       <c r="C160" s="29" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="64"/>
       <c r="B161" s="8"/>
       <c r="C161" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A162" s="64"/>
       <c r="B162" s="8"/>
       <c r="C162" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="65" t="s">
         <v>76</v>
       </c>
@@ -7456,7 +7462,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="65"/>
       <c r="B164" s="8"/>
       <c r="C164" s="31" t="s">
@@ -7472,7 +7478,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="65"/>
       <c r="B165" s="8" t="s">
         <v>41</v>
@@ -7490,7 +7496,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="261" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" ht="300" x14ac:dyDescent="0.25">
       <c r="A166" s="65"/>
       <c r="B166" s="8" t="s">
         <v>177</v>
@@ -7508,7 +7514,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A167" s="65"/>
       <c r="B167" s="8" t="s">
         <v>178</v>
@@ -7518,7 +7524,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="65"/>
       <c r="B168" s="15" t="s">
         <v>47</v>
@@ -7528,7 +7534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A169" s="65"/>
       <c r="B169" s="13" t="s">
         <v>52</v>
@@ -7538,7 +7544,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="65" t="s">
         <v>78</v>
       </c>
@@ -7561,7 +7567,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="65"/>
       <c r="B171" s="8"/>
       <c r="C171" s="46"/>
@@ -7571,7 +7577,7 @@
       <c r="E171" s="46"/>
       <c r="F171" s="46"/>
     </row>
-    <row r="172" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="65"/>
       <c r="B172" s="8" t="s">
         <v>41</v>
@@ -7589,7 +7595,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A173" s="65"/>
       <c r="B173" s="8" t="s">
         <v>177</v>
@@ -7607,7 +7613,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A174" s="65"/>
       <c r="B174" s="8" t="s">
         <v>179</v>
@@ -7617,7 +7623,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A175" s="65"/>
       <c r="B175" s="15" t="s">
         <v>47</v>
@@ -7627,7 +7633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A176" s="65"/>
       <c r="B176" s="13" t="s">
         <v>52</v>
@@ -7637,7 +7643,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="65" t="s">
         <v>80</v>
       </c>
@@ -7660,7 +7666,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="65"/>
       <c r="B178" s="8" t="s">
         <v>41</v>
@@ -7678,7 +7684,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A179" s="65"/>
       <c r="B179" s="8" t="s">
         <v>177</v>
@@ -7696,28 +7702,28 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A180" s="65"/>
       <c r="B180" s="8" t="s">
         <v>180</v>
       </c>
       <c r="C180" s="29"/>
     </row>
-    <row r="181" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="65"/>
       <c r="B181" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C181" s="29"/>
     </row>
-    <row r="182" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="55"/>
       <c r="B182" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C182" s="29"/>
     </row>
-    <row r="183" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="65" t="s">
         <v>82</v>
       </c>
@@ -7740,7 +7746,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="65"/>
       <c r="B184" s="8" t="s">
         <v>41</v>
@@ -7758,7 +7764,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A185" s="65"/>
       <c r="B185" s="8" t="s">
         <v>177</v>
@@ -7776,13 +7782,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A186" s="65"/>
       <c r="B186" s="8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="65"/>
       <c r="B187" s="8" t="s">
         <v>47</v>
@@ -7791,7 +7797,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="65"/>
       <c r="B188" s="16" t="s">
         <v>52</v>
@@ -7800,133 +7806,143 @@
         <v>90</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="65"/>
       <c r="C189" s="29"/>
     </row>
-    <row r="190" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="57"/>
       <c r="C190" s="49"/>
     </row>
-    <row r="191" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="57"/>
     </row>
-    <row r="192" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="57"/>
     </row>
-    <row r="193" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="57"/>
     </row>
-    <row r="194" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="57"/>
     </row>
-    <row r="195" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="57"/>
     </row>
-    <row r="196" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="57"/>
     </row>
-    <row r="197" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="57"/>
     </row>
-    <row r="198" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="57"/>
     </row>
-    <row r="199" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="57"/>
     </row>
-    <row r="200" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="57"/>
     </row>
-    <row r="201" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="57"/>
     </row>
-    <row r="202" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="57"/>
     </row>
-    <row r="203" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="57"/>
     </row>
-    <row r="204" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="57"/>
     </row>
-    <row r="205" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="57"/>
     </row>
-    <row r="206" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="57"/>
     </row>
-    <row r="207" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="57"/>
     </row>
-    <row r="208" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="57"/>
     </row>
-    <row r="209" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="57"/>
     </row>
-    <row r="210" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="57"/>
     </row>
-    <row r="211" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="57"/>
     </row>
-    <row r="212" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="57"/>
     </row>
-    <row r="213" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="57"/>
     </row>
-    <row r="214" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="57"/>
     </row>
-    <row r="215" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="57"/>
     </row>
-    <row r="216" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="57"/>
     </row>
-    <row r="217" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="57"/>
     </row>
-    <row r="218" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="57"/>
     </row>
-    <row r="219" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="57"/>
     </row>
-    <row r="220" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="57"/>
     </row>
-    <row r="221" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="57"/>
     </row>
-    <row r="222" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="57"/>
     </row>
-    <row r="223" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="57"/>
     </row>
-    <row r="224" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="57"/>
     </row>
-    <row r="225" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="57"/>
     </row>
-    <row r="226" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="57"/>
     </row>
-    <row r="227" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="57"/>
     </row>
-    <row r="228" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="57"/>
     </row>
-    <row r="229" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A183:A189"/>
     <mergeCell ref="A59:A62"/>
@@ -7942,16 +7958,6 @@
     <mergeCell ref="A170:A176"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>